<commit_message>
updates all help dialogs to new format, content unchanged
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/symbolic.xlsx
+++ b/doc/help_dialogs/Input_files/symbolic.xlsx
@@ -920,7 +920,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
-update help system to use external files
-xlsx_to_artisan_help.py generates more efficient output files, plus other fixes
-move autosave help button to be consistent with other dialogs
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/symbolic.xlsx
+++ b/doc/help_dialogs/Input_files/symbolic.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="158">
   <si>
     <t>SYMBOLIC VARIABLES</t>
   </si>
@@ -486,6 +486,18 @@
   </si>
   <si>
     <t>ET value delayed by 2 indexes</t>
+  </si>
+  <si>
+    <t>RB1</t>
+  </si>
+  <si>
+    <t>RB2</t>
+  </si>
+  <si>
+    <t>Background ET rate of rise</t>
+  </si>
+  <si>
+    <t>Background BT rate of rise</t>
   </si>
 </sst>
 </file>
@@ -584,7 +596,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -605,13 +617,23 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -920,9 +942,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -932,316 +952,337 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
     </row>
     <row r="2" spans="1:3" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="12" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="3"/>
+      <c r="C5" s="12"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="C19" s="3"/>
+      <c r="C19" s="12"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="3"/>
+      <c r="C20" s="12"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="3"/>
+      <c r="C21" s="12"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="C22" s="3"/>
+      <c r="C22" s="12"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="C23" s="3"/>
+      <c r="C23" s="12"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
+      <c r="A24" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="3"/>
+      <c r="C24" s="12"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="C25" s="3"/>
+      <c r="C25" s="12"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="C26" s="3"/>
+      <c r="C26" s="12"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="7" t="s">
+      <c r="A27" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="C27" s="3"/>
+      <c r="C27" s="12"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="7" t="s">
+      <c r="A28" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="C28" s="3"/>
+      <c r="C28" s="12"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="7"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
+      <c r="A29" s="13"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="12"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="7" t="s">
+      <c r="A30" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="7" t="s">
+      <c r="A31" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="12" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="5"/>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="5"/>
     </row>
   </sheetData>
@@ -1273,7 +1314,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="9" t="s">
         <v>93</v>
       </c>
       <c r="B3">
@@ -1281,7 +1322,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="9" t="s">
         <v>94</v>
       </c>
       <c r="B4">
@@ -1323,7 +1364,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="9" t="s">
         <v>141</v>
       </c>
       <c r="B4" t="s">
@@ -1331,7 +1372,7 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="9" t="s">
         <v>142</v>
       </c>
       <c r="B5" t="s">
@@ -1430,7 +1471,7 @@
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="8" t="s">
         <v>151</v>
       </c>
       <c r="B11" s="6" t="s">
@@ -1506,7 +1547,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="9" t="s">
         <v>104</v>
       </c>
       <c r="B3" t="s">
@@ -1514,7 +1555,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="9" t="s">
         <v>106</v>
       </c>
       <c r="B4" t="s">
@@ -1555,7 +1596,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="9" t="s">
         <v>119</v>
       </c>
       <c r="B3" t="s">
@@ -1563,7 +1604,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="9" t="s">
         <v>120</v>
       </c>
       <c r="B4" t="s">
@@ -1571,7 +1612,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="9" t="s">
         <v>123</v>
       </c>
       <c r="B6" t="s">
@@ -1607,7 +1648,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="9" t="s">
         <v>125</v>
       </c>
       <c r="B3" t="s">
@@ -1615,7 +1656,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="9" t="s">
         <v>127</v>
       </c>
       <c r="B4" t="s">
@@ -1623,7 +1664,7 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="9" t="s">
         <v>126</v>
       </c>
       <c r="B5" t="s">
@@ -1659,7 +1700,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="9" t="s">
         <v>132</v>
       </c>
       <c r="B3" t="s">
@@ -1667,7 +1708,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="9" t="s">
         <v>133</v>
       </c>
       <c r="B4" t="s">
@@ -1731,7 +1772,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="9" t="s">
         <v>101</v>
       </c>
       <c r="B3" t="s">

</xml_diff>

<commit_message>
-typo in help file
-serial table improvement
-correct ext in saveVectorGraph
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/symbolic.xlsx
+++ b/doc/help_dialogs/Input_files/symbolic.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="150" windowWidth="20115" windowHeight="7995" tabRatio="876" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="150" windowWidth="20115" windowHeight="7995" tabRatio="876" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Symbolic Variables" sheetId="1" r:id="rId1"/>
@@ -422,9 +422,6 @@
     <t>pDRY</t>
   </si>
   <si>
-    <t>pFCS</t>
-  </si>
-  <si>
     <t>Prediction of the time distance to the DRY event based on the current RoR. Evaluates to -1 on negative RoR and to 0 if the DRY event is already set.</t>
   </si>
   <si>
@@ -498,6 +495,9 @@
   </si>
   <si>
     <t>bn:Note: RoR values r can be scaled to the temperature axis using a linear approximation of the form "r*k + o". As the variables k and o depend on the actual axis settings which can be changed by the user without triggering a recomputation, those variable are less useful for use in a recording, but useful in the Plotter to plot w.r.t. the RoR y-axis instead of the temperature y-axis.</t>
+  </si>
+  <si>
+    <t>pFCs</t>
   </si>
 </sst>
 </file>
@@ -1262,10 +1262,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C32" s="12" t="s">
         <v>5</v>
@@ -1273,10 +1273,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C33" s="12" t="s">
         <v>5</v>
@@ -1365,7 +1365,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B4" t="s">
         <v>114</v>
@@ -1373,7 +1373,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B5" t="s">
         <v>115</v>
@@ -1416,7 +1416,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>2</v>
@@ -1427,7 +1427,7 @@
         <v>59</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1443,7 +1443,7 @@
         <v>57</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
@@ -1451,7 +1451,7 @@
         <v>58</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1459,7 +1459,7 @@
         <v>62</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
@@ -1467,15 +1467,15 @@
         <v>63</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>150</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -1495,7 +1495,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1508,10 +1508,10 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -1523,7 +1523,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -1564,7 +1564,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -1680,8 +1680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1704,40 +1704,40 @@
         <v>131</v>
       </c>
       <c r="B3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>132</v>
+        <v>157</v>
       </c>
       <c r="B4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- updates CTE MODBUS TCP machine setups - adds control to Diedrich DR machine setup and adds Diedrich CR machine setup - adds (total) correction to cup profiles and enables column drag-and-drop
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/symbolic.xlsx
+++ b/doc/help_dialogs/Input_files/symbolic.xlsx
@@ -526,7 +526,7 @@
     <t xml:space="preserve">bit(n,x)</t>
   </si>
   <si>
-    <t xml:space="preserve">Return1 if the bit n of value x (interpreted as integer) is set.</t>
+    <t xml:space="preserve">Return 1 if the bit n of value x (interpreted as integer) is set, otherwise 0.</t>
   </si>
   <si>
     <t xml:space="preserve">MATHEMATICAL CONSTANTS</t>
@@ -819,7 +819,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="59.82"/>
@@ -1180,7 +1180,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="44.09"/>
   </cols>
@@ -1228,7 +1228,7 @@
       <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.09"/>
@@ -1367,7 +1367,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="26.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="38.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="8" t="s">
         <v>163</v>
       </c>
@@ -1397,7 +1397,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -1450,7 +1450,7 @@
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -1508,10 +1508,10 @@
       <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1616,7 +1616,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -1661,10 +1661,10 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.11"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1723,7 +1723,7 @@
       <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -1784,7 +1784,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -1845,7 +1845,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -1923,7 +1923,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -1989,7 +1989,7 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">

</xml_diff>